<commit_message>
change swr computation to voltage instead of power since detectors are in square law range, fix more bugs and return to coarse/fine tune algorithm, speed up relay, swr measure
</commit_message>
<xml_diff>
--- a/Arduino_tuner/Power_cal.xlsx
+++ b/Arduino_tuner/Power_cal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\Arduino_tuner\Arduino_tuner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83946746-79D4-4B82-9BE2-9DA8CADAD414}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4376B9AC-2125-49D3-84AC-30D1C38ABBC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15460" xr2:uid="{D348E346-242F-4A8E-BF56-F653B9B22A6A}"/>
+    <workbookView xWindow="6310" yWindow="3780" windowWidth="28800" windowHeight="15460" xr2:uid="{D348E346-242F-4A8E-BF56-F653B9B22A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,749 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>detector</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> output vs root of power</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>820</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2360679774997898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1622776601683795</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4721359549995796</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.4772255750516612</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.324555320336759</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0710678118654755</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.745966692414834</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.3666002653407556</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.9442719099991592</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.4868329805051381</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EC81-4594-92D9-5AA238C4A56D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="479348184"/>
+        <c:axId val="479347856"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$1:$A$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>159</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>230</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>330</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>420</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>490</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>565</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>620</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>670</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>720</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>780</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>820</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$1:$C$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.2360679774997898</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3.1622776601683795</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4.4721359549995796</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5.4772255750516612</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6.324555320336759</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7.0710678118654755</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7.745966692414834</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8.3666002653407556</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>8.9442719099991592</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>9.4868329805051381</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000E-EC81-4594-92D9-5AA238C4A56D}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$1:$A$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>159</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>230</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>330</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>420</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>490</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>565</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>620</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>670</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>720</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>780</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>820</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$1:$C$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.2360679774997898</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3.1622776601683795</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4.4721359549995796</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5.4772255750516612</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6.324555320336759</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7.0710678118654755</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7.745966692414834</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8.3666002653407556</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>8.9442719099991592</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>9.4868329805051381</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000F-EC81-4594-92D9-5AA238C4A56D}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="479348184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479347856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="479347856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479348184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1004,20 +1746,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>60325</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1037,6 +2295,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>320675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{723ABBC0-1063-491B-8E21-EFF667B5679E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1342,108 +2636,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BE6AED-459F-48E4-8F39-39D0D64C96C7}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
         <v>0</v>
       </c>
+      <c r="C1">
+        <f>SQRT(B1)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>159</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C12" si="0">SQRT(B2)</f>
+        <v>2.2360679774997898</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>230</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>3.1622776601683795</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>330</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>4.4721359549995796</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>420</v>
       </c>
       <c r="B5">
         <v>30</v>
       </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5.4772255750516612</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>490</v>
       </c>
       <c r="B6">
         <v>40</v>
       </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>6.324555320336759</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>565</v>
       </c>
       <c r="B7">
         <v>50</v>
       </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>7.0710678118654755</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>620</v>
       </c>
       <c r="B8">
         <v>60</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>7.745966692414834</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>670</v>
       </c>
       <c r="B9">
         <v>70</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>8.3666002653407556</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>720</v>
       </c>
       <c r="B10">
         <v>80</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>8.9442719099991592</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>780</v>
       </c>
       <c r="B11">
         <v>90</v>
       </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>9.4868329805051381</v>
+      </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>820</v>
       </c>
       <c r="B12">
         <v>100</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>